<commit_message>
+ abastract adaptor with base map methods + additional methods in TestDataObject interface + toMap tests with testdata (except mongo)
</commit_message>
<xml_diff>
--- a/src/test/resources/excell/TestData.xlsx
+++ b/src/test/resources/excell/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Описание</t>
   </si>
@@ -147,12 +147,48 @@
   </si>
   <si>
     <t>link:Tests.Common.gendata</t>
+  </si>
+  <si>
+    <t>MapTests</t>
+  </si>
+  <si>
+    <t>stringValue</t>
+  </si>
+  <si>
+    <t>This is simple string</t>
+  </si>
+  <si>
+    <t>singleCharValue</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>integerValue</t>
+  </si>
+  <si>
+    <t>floatValue</t>
+  </si>
+  <si>
+    <t>doubleValue</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -235,6 +271,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,6 +739,84 @@
       </c>
       <c r="D14" s="4"/>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="9">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="10">
+        <v>42.1</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="11">
+        <v>42.21</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -703,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>